<commit_message>
17.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Stock Imei/imei list.xlsx
+++ b/2020/Stock Imei/imei list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>R40</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>bl97</t>
+  </si>
+  <si>
+    <t>i15</t>
+  </si>
+  <si>
+    <t>z25</t>
+  </si>
+  <si>
+    <t>bl60</t>
   </si>
 </sst>
 </file>
@@ -427,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,8 +446,8 @@
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="11" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="14" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" s="2" customFormat="1">
@@ -475,6 +484,15 @@
       <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:65">
       <c r="A2" s="3">
@@ -508,9 +526,15 @@
       <c r="K2" s="3">
         <v>357655105048441</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="L2" s="3">
+        <v>357651101395241</v>
+      </c>
+      <c r="M2" s="3">
+        <v>351918111257661</v>
+      </c>
+      <c r="N2" s="3">
+        <v>353515112106828</v>
+      </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -585,7 +609,9 @@
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="N3" s="3">
+        <v>353515112117809</v>
+      </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -660,7 +686,9 @@
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="N4" s="3">
+        <v>353515112099809</v>
+      </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -730,7 +758,9 @@
         <v>359998102939321</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>357655105939623</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -1574,7 +1604,9 @@
       <c r="D17" s="3">
         <v>359152107936789</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>359777106739642</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1643,7 +1675,9 @@
       <c r="D18" s="3">
         <v>359152108572922</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>359777107011629</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1712,7 +1746,9 @@
       <c r="D19" s="3">
         <v>359152108573649</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3">
+        <v>359777106967862</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1781,7 +1817,9 @@
       <c r="D20" s="3">
         <v>359152108617743</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>359777106807803</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -1850,7 +1888,9 @@
       <c r="D21" s="3">
         <v>359152108573185</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3">
+        <v>359777107008468</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1985,7 +2025,9 @@
       <c r="A23" s="3"/>
       <c r="B23" s="5"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3">
+        <v>359152107529881</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -2052,7 +2094,9 @@
       <c r="A24" s="3"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3">
+        <v>359152107530467</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>

</xml_diff>

<commit_message>
19.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Stock Imei/imei list.xlsx
+++ b/2020/Stock Imei/imei list.xlsx
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,7 +696,9 @@
       <c r="J3" s="3">
         <v>359998103191005</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3">
+        <v>353428110199248</v>
+      </c>
       <c r="L3" s="3">
         <v>357655105058945</v>
       </c>
@@ -1248,7 +1250,9 @@
     <row r="10" spans="1:66">
       <c r="A10" s="3"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5">
+        <v>358444100836343</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3">
         <v>359152107940526</v>
@@ -1324,7 +1328,9 @@
     <row r="11" spans="1:66">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>358444100822988</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3">
         <v>359152107937688</v>
@@ -2364,7 +2370,9 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3">
+        <v>359152108500725</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -2432,7 +2440,9 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3">
+        <v>359152108502903</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -2500,7 +2510,9 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3">
+        <v>359152108500667</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2568,7 +2580,9 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3">
+        <v>359152108500584</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>

</xml_diff>

<commit_message>
22.05.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Stock Imei/imei list.xlsx
+++ b/2020/Stock Imei/imei list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>R40</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>i95</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>i74</t>
   </si>
 </sst>
 </file>
@@ -506,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BN613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,8 +527,8 @@
     <col min="18" max="18" width="9.140625" style="1"/>
     <col min="19" max="19" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.140625" style="1"/>
-    <col min="21" max="25" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="1"/>
+    <col min="21" max="26" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" s="2" customFormat="1">
@@ -594,6 +600,9 @@
       </c>
       <c r="Y1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:66">
@@ -1535,7 +1544,9 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -2058,9 +2069,7 @@
       <c r="E20" s="3">
         <v>359152108617743</v>
       </c>
-      <c r="F20" s="3">
-        <v>359777106807803</v>
-      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -2132,9 +2141,7 @@
       <c r="E21" s="3">
         <v>359152108573185</v>
       </c>
-      <c r="F21" s="3">
-        <v>359777107008468</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>

</xml_diff>